<commit_message>
added Execute option and fixed SVI IP
</commit_message>
<xml_diff>
--- a/script_template.xlsx
+++ b/script_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamah/Programming/gtaa_N7K/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamah/Programming/gtaa_nexus7k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{00462528-E8C7-5741-A654-9D5B315DC520}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7C5B487B-53FA-4441-B7F7-1BC8ABB303B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="15100" windowWidth="42900" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="7500" windowWidth="42900" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>de Guzman,Christian</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5871EF22-B409-874B-B240-653E7B92ADA8}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{5871EF22-B409-874B-B240-653E7B92ADA8}">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{4331FAC6-6EBC-824D-9DBF-B1EF50800DD1}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{4331FAC6-6EBC-824D-9DBF-B1EF50800DD1}">
       <text>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{772885B1-4A72-3D40-A9B5-C359FE23D879}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{772885B1-4A72-3D40-A9B5-C359FE23D879}">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4534C310-5451-A149-8D9E-8240231D897E}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{4534C310-5451-A149-8D9E-8240231D897E}">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{C2EE775E-5143-884B-B9B1-2655D874FFDA}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{C2EE775E-5143-884B-B9B1-2655D874FFDA}">
       <text>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{3BCAC494-2050-9A49-8DA1-6F9A83E26D9B}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{3BCAC494-2050-9A49-8DA1-6F9A83E26D9B}">
       <text>
         <r>
           <rPr>
@@ -288,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{E2BAC1E5-5C1C-764D-AF05-640E49A6D196}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{E2BAC1E5-5C1C-764D-AF05-640E49A6D196}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{9845FE0B-CA87-A04F-B200-DBD284D21E9D}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{9845FE0B-CA87-A04F-B200-DBD284D21E9D}">
       <text>
         <r>
           <rPr>
@@ -385,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{57C15850-50D1-8E49-959D-DD0D1C5A100D}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{57C15850-50D1-8E49-959D-DD0D1C5A100D}">
       <text>
         <r>
           <rPr>
@@ -428,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{69BF626E-3DD2-AF47-A91C-F03E822E2D2E}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{69BF626E-3DD2-AF47-A91C-F03E822E2D2E}">
       <text>
         <r>
           <rPr>
@@ -456,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{569B2A97-8AC7-124A-ACA8-1178A9C4ABBF}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{569B2A97-8AC7-124A-ACA8-1178A9C4ABBF}">
       <text>
         <r>
           <rPr>
@@ -549,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{14FB83B2-EB8D-9740-93DA-935A831AD828}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{14FB83B2-EB8D-9740-93DA-935A831AD828}">
       <text>
         <r>
           <rPr>
@@ -642,7 +642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{8E871E6C-FB50-6340-BD36-310C26F3AD45}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{8E871E6C-FB50-6340-BD36-310C26F3AD45}">
       <text>
         <r>
           <rPr>
@@ -685,7 +685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{89C30FB3-7F4B-9340-AADE-99ED1F4BD53A}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{89C30FB3-7F4B-9340-AADE-99ED1F4BD53A}">
       <text>
         <r>
           <rPr>
@@ -710,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{BD0BE63D-4C6A-E24C-830B-75EB763C10B8}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{BD0BE63D-4C6A-E24C-830B-75EB763C10B8}">
       <text>
         <r>
           <rPr>
@@ -783,7 +783,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{D1A00FC7-5F69-9F42-ADAA-CD77B19E2EC5}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{D1A00FC7-5F69-9F42-ADAA-CD77B19E2EC5}">
       <text>
         <r>
           <rPr>
@@ -876,7 +876,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{4BE0F97A-8DB8-6845-8286-A4CA39751990}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{4BE0F97A-8DB8-6845-8286-A4CA39751990}">
       <text>
         <r>
           <rPr>
@@ -969,7 +969,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{F8B8875C-2D5B-A44C-B371-7E42D38BFACF}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{F8B8875C-2D5B-A44C-B371-7E42D38BFACF}">
       <text>
         <r>
           <rPr>
@@ -994,7 +994,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{88407990-8ABD-1146-8FE3-B85F786E7BA6}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{88407990-8ABD-1146-8FE3-B85F786E7BA6}">
       <text>
         <r>
           <rPr>
@@ -1019,7 +1019,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{FF7843A4-8627-7B4B-8C99-58A861FA1EFA}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{FF7843A4-8627-7B4B-8C99-58A861FA1EFA}">
       <text>
         <r>
           <rPr>
@@ -1047,7 +1047,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{BB1373D0-158F-2848-9503-2D6B21C9A763}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{BB1373D0-158F-2848-9503-2D6B21C9A763}">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{83E4E2DB-D267-594C-ABAF-594E63CD1B79}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{83E4E2DB-D267-594C-ABAF-594E63CD1B79}">
       <text>
         <r>
           <rPr>
@@ -1170,7 +1170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{788152CC-7D46-EE40-BB8F-EB7351A1CD1F}">
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{788152CC-7D46-EE40-BB8F-EB7351A1CD1F}">
       <text>
         <r>
           <rPr>
@@ -1195,7 +1195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{16925113-CF20-F840-A528-FCAFA8D83095}">
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{16925113-CF20-F840-A528-FCAFA8D83095}">
       <text>
         <r>
           <rPr>
@@ -1220,7 +1220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{F7C634E0-D1D9-9C44-9C19-E37EF66146FA}">
+    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{F7C634E0-D1D9-9C44-9C19-E37EF66146FA}">
       <text>
         <r>
           <rPr>
@@ -1248,7 +1248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{8047B7EA-AF6B-6E4A-B028-D7C0E15FFFC1}">
+    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{8047B7EA-AF6B-6E4A-B028-D7C0E15FFFC1}">
       <text>
         <r>
           <rPr>
@@ -1341,7 +1341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{BD314D32-0738-C04A-86FE-BACFEF4264AD}">
+    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{BD314D32-0738-C04A-86FE-BACFEF4264AD}">
       <text>
         <r>
           <rPr>
@@ -1371,7 +1371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{ED2D12BF-706F-AF4F-8346-B9D53CE88109}">
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{ED2D12BF-706F-AF4F-8346-B9D53CE88109}">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{61225CCE-92F0-6349-AC04-C85BCFBA3B7F}">
+    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{61225CCE-92F0-6349-AC04-C85BCFBA3B7F}">
       <text>
         <r>
           <rPr>
@@ -1457,67 +1457,67 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{0A7D56DD-43CB-A443-B0D0-4AA02F0E42DB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>de Guzman,Christian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{0A7D56DD-43CB-A443-B0D0-4AA02F0E42DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>ip prefix-list KE-CARGO-BO_GREY-MGMT_PFL permit 172.16.2.26/29 le 32</t>
         </r>
       </text>
     </comment>
-    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{CB809492-140F-5443-ADA9-5D9CAB367BF0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>de Guzman,Christian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="AK2" authorId="0" shapeId="0" xr:uid="{CB809492-140F-5443-ADA9-5D9CAB367BF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">route-map GREY-MGMT_KE-CARGO-BO permit 10
 </t>
@@ -1527,7 +1527,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">  match ip address prefix-list KE-CARGO-BO_GREY-MGMT_PFL 
 </t>
@@ -1537,40 +1537,40 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">  set extcommunity rt 65001:103 additive </t>
         </r>
       </text>
     </comment>
-    <comment ref="AK2" authorId="0" shapeId="0" xr:uid="{49C3CA03-760D-034C-8D4B-792255B0E98D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>de Guzman,Christian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="AL2" authorId="0" shapeId="0" xr:uid="{49C3CA03-760D-034C-8D4B-792255B0E98D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">vrf context KE-CARGO-BO
 </t>
@@ -1580,7 +1580,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">  address-family ipv4 unicast
 </t>
@@ -1590,13 +1590,13 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">    export map GREY-MGMT_KE-CARGO-BO</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{BB6E4A01-3467-3D41-B2B9-521499480F4A}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{BB6E4A01-3467-3D41-B2B9-521499480F4A}">
       <text>
         <r>
           <rPr>
@@ -1669,7 +1669,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{5AEA886C-59A6-9C42-87BA-04142F8BAFC8}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{5AEA886C-59A6-9C42-87BA-04142F8BAFC8}">
       <text>
         <r>
           <rPr>
@@ -1702,7 +1702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{27A6586C-F8FE-D944-9439-F44BB234E86A}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{27A6586C-F8FE-D944-9439-F44BB234E86A}">
       <text>
         <r>
           <rPr>
@@ -1735,7 +1735,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{CBF64C6A-7A73-8145-86C6-F6C623A5DD6E}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{CBF64C6A-7A73-8145-86C6-F6C623A5DD6E}">
       <text>
         <r>
           <rPr>
@@ -1788,7 +1788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{5EE65EFC-0F91-8548-AB43-9C0066E37BD4}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{5EE65EFC-0F91-8548-AB43-9C0066E37BD4}">
       <text>
         <r>
           <rPr>
@@ -1821,7 +1821,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{B422DCCD-5E1C-8F44-BA86-5ADD946E95B8}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{B422DCCD-5E1C-8F44-BA86-5ADD946E95B8}">
       <text>
         <r>
           <rPr>
@@ -1854,7 +1854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{E5FD6976-28D9-FB43-85EC-4DDB0255B882}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{E5FD6976-28D9-FB43-85EC-4DDB0255B882}">
       <text>
         <r>
           <rPr>
@@ -1908,7 +1908,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{71A4C170-1858-E142-ABF8-507476D44EC4}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{71A4C170-1858-E142-ABF8-507476D44EC4}">
       <text>
         <r>
           <rPr>
@@ -1951,7 +1951,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{EF3A977E-0C1A-9F49-B83D-0A5F4AC1459F}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{EF3A977E-0C1A-9F49-B83D-0A5F4AC1459F}">
       <text>
         <r>
           <rPr>
@@ -1994,7 +1994,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{AB2D94E6-4992-EF43-93A1-760C22FC2139}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{AB2D94E6-4992-EF43-93A1-760C22FC2139}">
       <text>
         <r>
           <rPr>
@@ -2022,7 +2022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{77FD2A32-1DEF-8A44-B35C-E3FF94969678}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{77FD2A32-1DEF-8A44-B35C-E3FF94969678}">
       <text>
         <r>
           <rPr>
@@ -2115,7 +2115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{40264F35-A93F-E846-94B2-DB279BBE4C63}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{40264F35-A93F-E846-94B2-DB279BBE4C63}">
       <text>
         <r>
           <rPr>
@@ -2208,7 +2208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{304FB755-D328-7E42-895B-3AF092512D97}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{304FB755-D328-7E42-895B-3AF092512D97}">
       <text>
         <r>
           <rPr>
@@ -2251,7 +2251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{CA592A6D-B111-3D42-905A-DB9903D7B688}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{CA592A6D-B111-3D42-905A-DB9903D7B688}">
       <text>
         <r>
           <rPr>
@@ -2276,7 +2276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{5F27EE17-A6BC-3A44-8560-EE2EE3E6495C}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{5F27EE17-A6BC-3A44-8560-EE2EE3E6495C}">
       <text>
         <r>
           <rPr>
@@ -2349,7 +2349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{564EB85D-DD78-EE42-995F-BD1AD915AC3D}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{564EB85D-DD78-EE42-995F-BD1AD915AC3D}">
       <text>
         <r>
           <rPr>
@@ -2442,7 +2442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{F2D4F363-370A-EF49-A093-231D40E2E875}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{F2D4F363-370A-EF49-A093-231D40E2E875}">
       <text>
         <r>
           <rPr>
@@ -2535,7 +2535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{8BB51AEA-713F-C347-AA17-3091424787DA}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{8BB51AEA-713F-C347-AA17-3091424787DA}">
       <text>
         <r>
           <rPr>
@@ -2578,7 +2578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{C8BC871E-1EAC-B34D-9195-6D45270AF0E6}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{C8BC871E-1EAC-B34D-9195-6D45270AF0E6}">
       <text>
         <r>
           <rPr>
@@ -2603,7 +2603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{6A746EA6-708A-684F-8E4A-72E07474D9C0}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{6A746EA6-708A-684F-8E4A-72E07474D9C0}">
       <text>
         <r>
           <rPr>
@@ -2631,7 +2631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{778F1D0D-4305-1F41-BAE6-3DEA4AA7DD19}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{778F1D0D-4305-1F41-BAE6-3DEA4AA7DD19}">
       <text>
         <r>
           <rPr>
@@ -2724,7 +2724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{6072B4E3-77A1-2D46-93ED-27873E4FA5B9}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{6072B4E3-77A1-2D46-93ED-27873E4FA5B9}">
       <text>
         <r>
           <rPr>
@@ -2754,7 +2754,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{8D7BDD2C-AFE9-504F-93E4-5FB31771CFF8}">
+    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{8D7BDD2C-AFE9-504F-93E4-5FB31771CFF8}">
       <text>
         <r>
           <rPr>
@@ -2779,7 +2779,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{8888DADC-8829-CB45-8197-F3DAD88FFC96}">
+    <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{8888DADC-8829-CB45-8197-F3DAD88FFC96}">
       <text>
         <r>
           <rPr>
@@ -2804,7 +2804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{3139D989-394D-B245-8AB8-D39A40E5E074}">
+    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{3139D989-394D-B245-8AB8-D39A40E5E074}">
       <text>
         <r>
           <rPr>
@@ -2832,7 +2832,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{19CF13E2-951A-C849-8096-A1DBAA004A67}">
+    <comment ref="AE3" authorId="0" shapeId="0" xr:uid="{19CF13E2-951A-C849-8096-A1DBAA004A67}">
       <text>
         <r>
           <rPr>
@@ -2925,7 +2925,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF3" authorId="0" shapeId="0" xr:uid="{617E7B30-C15A-A447-B517-92F4D3A05D00}">
+    <comment ref="AG3" authorId="0" shapeId="0" xr:uid="{617E7B30-C15A-A447-B517-92F4D3A05D00}">
       <text>
         <r>
           <rPr>
@@ -3018,7 +3018,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG3" authorId="0" shapeId="0" xr:uid="{37938625-75C9-9B45-9722-1CEA64CEDC8C}">
+    <comment ref="AH3" authorId="0" shapeId="0" xr:uid="{37938625-75C9-9B45-9722-1CEA64CEDC8C}">
       <text>
         <r>
           <rPr>
@@ -3051,7 +3051,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH3" authorId="0" shapeId="0" xr:uid="{B2DEB61C-2991-CF44-8505-24A5634D7EF8}">
+    <comment ref="AI3" authorId="0" shapeId="0" xr:uid="{B2DEB61C-2991-CF44-8505-24A5634D7EF8}">
       <text>
         <r>
           <rPr>
@@ -3104,67 +3104,67 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI3" authorId="0" shapeId="0" xr:uid="{F223696E-6A84-BC4F-80AD-A4FD7859122C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>de Guzman,Christian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="AJ3" authorId="0" shapeId="0" xr:uid="{F223696E-6A84-BC4F-80AD-A4FD7859122C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>ip prefix-list KE-CARGO-BO_GREY-MGMT_PFL permit 172.16.2.26/29 le 32</t>
         </r>
       </text>
     </comment>
-    <comment ref="AJ3" authorId="0" shapeId="0" xr:uid="{507B6F06-0DBB-1647-B1D2-3ADC8766BF8F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>de Guzman,Christian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="AK3" authorId="0" shapeId="0" xr:uid="{507B6F06-0DBB-1647-B1D2-3ADC8766BF8F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">route-map GREY-MGMT_KE-CARGO-BO permit 10
 </t>
@@ -3174,7 +3174,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">  match ip address prefix-list KE-CARGO-BO_GREY-MGMT_PFL 
 </t>
@@ -3184,40 +3184,40 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">  set extcommunity rt 65001:103 additive </t>
         </r>
       </text>
     </comment>
-    <comment ref="AK3" authorId="0" shapeId="0" xr:uid="{DA3CE0FE-308F-D241-86F3-21535A9549F9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>de Guzman,Christian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="AL3" authorId="0" shapeId="0" xr:uid="{DA3CE0FE-308F-D241-86F3-21535A9549F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>de Guzman,Christian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">vrf context KE-CARGO-BO
 </t>
@@ -3227,7 +3227,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">  address-family ipv4 unicast
 </t>
@@ -3237,13 +3237,13 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">    export map GREY-MGMT_KE-CARGO-BO</t>
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{2850C7EA-C7E0-F548-A46E-35AEC1269302}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{2850C7EA-C7E0-F548-A46E-35AEC1269302}">
       <text>
         <r>
           <rPr>
@@ -3276,7 +3276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{35CD00B9-C7B9-9246-BAE5-BD2F8AA58C3A}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{35CD00B9-C7B9-9246-BAE5-BD2F8AA58C3A}">
       <text>
         <r>
           <rPr>
@@ -3329,7 +3329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{1EFD9A2D-E46E-6F49-8648-A88B64C73818}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{1EFD9A2D-E46E-6F49-8648-A88B64C73818}">
       <text>
         <r>
           <rPr>
@@ -3362,7 +3362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{64176847-409B-2B4D-BF08-DB95789FD971}">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{64176847-409B-2B4D-BF08-DB95789FD971}">
       <text>
         <r>
           <rPr>
@@ -3416,7 +3416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{094D8AF0-EA18-DF4E-8767-7C3083AB23C3}">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{094D8AF0-EA18-DF4E-8767-7C3083AB23C3}">
       <text>
         <r>
           <rPr>
@@ -3459,7 +3459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{7DEB5F41-3809-E042-A41D-CE5022FFEC23}">
+    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{7DEB5F41-3809-E042-A41D-CE5022FFEC23}">
       <text>
         <r>
           <rPr>
@@ -3502,7 +3502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{FFB5FB5D-25C2-2544-816F-C589089146A7}">
+    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{FFB5FB5D-25C2-2544-816F-C589089146A7}">
       <text>
         <r>
           <rPr>
@@ -3575,7 +3575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{C3AD692B-2E1D-A943-AF06-6E3DB7CBC24C}">
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{C3AD692B-2E1D-A943-AF06-6E3DB7CBC24C}">
       <text>
         <r>
           <rPr>
@@ -3668,7 +3668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{30FAD6D2-A92D-7540-876C-3495E752EFB6}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{30FAD6D2-A92D-7540-876C-3495E752EFB6}">
       <text>
         <r>
           <rPr>
@@ -3761,7 +3761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U4" authorId="0" shapeId="0" xr:uid="{D005327D-D825-3C4D-8394-05B8B0C10F56}">
+    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{D005327D-D825-3C4D-8394-05B8B0C10F56}">
       <text>
         <r>
           <rPr>
@@ -3786,7 +3786,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{C22AB09C-1D1F-A645-B056-F5B19E9D2DF9}">
+    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{C22AB09C-1D1F-A645-B056-F5B19E9D2DF9}">
       <text>
         <r>
           <rPr>
@@ -3811,7 +3811,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W4" authorId="0" shapeId="0" xr:uid="{5CD5E383-CD38-8940-AA53-66D737593B35}">
+    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{5CD5E383-CD38-8940-AA53-66D737593B35}">
       <text>
         <r>
           <rPr>
@@ -3839,7 +3839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{863CDDAB-8338-C24D-8F94-381E3D93E173}">
+    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{863CDDAB-8338-C24D-8F94-381E3D93E173}">
       <text>
         <r>
           <rPr>
@@ -3932,7 +3932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z4" authorId="0" shapeId="0" xr:uid="{B4BCA3A2-3E0D-834D-81A6-49F3E1BCF5C5}">
+    <comment ref="AA4" authorId="0" shapeId="0" xr:uid="{B4BCA3A2-3E0D-834D-81A6-49F3E1BCF5C5}">
       <text>
         <r>
           <rPr>
@@ -3962,7 +3962,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{B7C8DDF2-BC1B-B145-A027-560A157F11F5}">
+    <comment ref="AH4" authorId="0" shapeId="0" xr:uid="{B7C8DDF2-BC1B-B145-A027-560A157F11F5}">
       <text>
         <r>
           <rPr>
@@ -3995,7 +3995,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{31A528BC-61B8-914D-A811-C2DABD64335C}">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{31A528BC-61B8-914D-A811-C2DABD64335C}">
       <text>
         <r>
           <rPr>
@@ -4028,7 +4028,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{9A9436BD-B50A-B147-8FE1-05395D419C58}">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{9A9436BD-B50A-B147-8FE1-05395D419C58}">
       <text>
         <r>
           <rPr>
@@ -4081,7 +4081,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{C4CC7D91-8705-994A-AACA-16DBE344E58E}">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{C4CC7D91-8705-994A-AACA-16DBE344E58E}">
       <text>
         <r>
           <rPr>
@@ -4124,7 +4124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{57778700-CC44-0E41-96AA-6D4B4DFD600E}">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{57778700-CC44-0E41-96AA-6D4B4DFD600E}">
       <text>
         <r>
           <rPr>
@@ -4167,7 +4167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{BAA6E14D-2237-B64A-86A2-23B357E00955}">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{BAA6E14D-2237-B64A-86A2-23B357E00955}">
       <text>
         <r>
           <rPr>
@@ -4240,7 +4240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{1FB581D7-3D92-D54A-B55C-FA486A93922C}">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{1FB581D7-3D92-D54A-B55C-FA486A93922C}">
       <text>
         <r>
           <rPr>
@@ -4333,7 +4333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{3E015D7C-2CA4-CA49-9E53-3868B0C29C6E}">
+    <comment ref="U5" authorId="0" shapeId="0" xr:uid="{3E015D7C-2CA4-CA49-9E53-3868B0C29C6E}">
       <text>
         <r>
           <rPr>
@@ -4426,7 +4426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA5" authorId="0" shapeId="0" xr:uid="{AB0C632D-D1F6-AD43-B22F-26685E27AE00}">
+    <comment ref="AB5" authorId="0" shapeId="0" xr:uid="{AB0C632D-D1F6-AD43-B22F-26685E27AE00}">
       <text>
         <r>
           <rPr>
@@ -4451,7 +4451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB5" authorId="0" shapeId="0" xr:uid="{2E3C0998-2566-D04D-AB53-857FC2BB9A1E}">
+    <comment ref="AC5" authorId="0" shapeId="0" xr:uid="{2E3C0998-2566-D04D-AB53-857FC2BB9A1E}">
       <text>
         <r>
           <rPr>
@@ -4476,7 +4476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC5" authorId="0" shapeId="0" xr:uid="{27493DBC-D7C1-0847-A8DB-4B276D4FD055}">
+    <comment ref="AD5" authorId="0" shapeId="0" xr:uid="{27493DBC-D7C1-0847-A8DB-4B276D4FD055}">
       <text>
         <r>
           <rPr>
@@ -4504,7 +4504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD5" authorId="0" shapeId="0" xr:uid="{06F3D1E5-A41F-4E4C-888E-14A229ED852F}">
+    <comment ref="AE5" authorId="0" shapeId="0" xr:uid="{06F3D1E5-A41F-4E4C-888E-14A229ED852F}">
       <text>
         <r>
           <rPr>
@@ -4597,7 +4597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF5" authorId="0" shapeId="0" xr:uid="{1095E351-1800-7A4B-9A53-2F8D017F452E}">
+    <comment ref="AG5" authorId="0" shapeId="0" xr:uid="{1095E351-1800-7A4B-9A53-2F8D017F452E}">
       <text>
         <r>
           <rPr>
@@ -4690,7 +4690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG5" authorId="0" shapeId="0" xr:uid="{FBA4A363-1ACA-DD46-A752-054BBF61E76A}">
+    <comment ref="AH5" authorId="0" shapeId="0" xr:uid="{FBA4A363-1ACA-DD46-A752-054BBF61E76A}">
       <text>
         <r>
           <rPr>
@@ -4728,7 +4728,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
     <t>RD</t>
   </si>
@@ -4942,13 +4942,16 @@
   </si>
   <si>
     <t>GREY</t>
+  </si>
+  <si>
+    <t>Execute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4981,19 +4984,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -5389,488 +5379,504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3">
         <v>2177</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>7</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>111</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="9">
+      <c r="S2" s="9">
         <v>106</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="10">
+      <c r="Y2" s="10">
         <v>110</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AB2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="11" t="s">
+      <c r="AC2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="11">
+      <c r="AE2" s="11">
         <v>108</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AF2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="AK2" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="AL2" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3">
         <v>2400</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>6</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>112</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="9">
+      <c r="S3" s="9">
         <v>105</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="U3" s="10"/>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
       <c r="Y3" s="10"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="11"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="1"/>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
       <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="3" t="s">
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>23</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="AK3" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="AL3" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:37" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3">
         <v>2222</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>5</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>111</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="10">
+      <c r="Y4" s="10">
         <v>110</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Z4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
         <v>2225</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>3</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="9">
+      <c r="S5" s="9">
         <v>105</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AA5" s="11" t="s">
+      <c r="AB5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="11" t="s">
+      <c r="AC5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="AD5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AD5" s="11">
+      <c r="AE5" s="11">
         <v>108</v>
       </c>
-      <c r="AE5" s="11" t="s">
+      <c r="AF5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>